<commit_message>
Atualizado com criação de planilha estática
</commit_message>
<xml_diff>
--- a/planilha.xlsx
+++ b/planilha.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="inf" r:id="rId3" sheetId="1"/>
+    <sheet name="adm" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -33,6 +34,15 @@
   </si>
   <si>
     <t>Nota Média</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -83,8 +93,202 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2"/>
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>